<commit_message>
Entrega da Fase 3
</commit_message>
<xml_diff>
--- a/docs/projeto-final/pesquisas/pesquisas.xlsx
+++ b/docs/projeto-final/pesquisas/pesquisas.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.barbosa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateusjbarbosa/Documents/Desenvolvimento/Repos/fai.etanois.docs/docs/projeto-final/pesquisas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFCEF80-0BEC-48A7-B524-0DB884728D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CF7AF-78A6-BB49-A2C2-4D6D75FEB4F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13140" xr2:uid="{D9E7E27E-ABC6-4427-AF05-B1E2A0954FEE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pesquisa #01 - Valores" sheetId="1" r:id="rId1"/>
+    <sheet name="Pesquisa #01 - Preços" sheetId="1" r:id="rId1"/>
     <sheet name="Pesquisa #02 - Funcionalidades" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -332,17 +332,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -361,7 +361,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -394,7 +394,7 @@
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Valores da Gasolina Comum</a:t>
+              <a:t>Preços da Gasolina Comum</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" b="1" baseline="0">
@@ -434,7 +434,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -449,7 +449,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$6</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -484,9 +484,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$5:$Q$5</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$5:$Q$5</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -538,7 +538,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$6:$Q$6</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$6:$Q$6</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="15"/>
@@ -602,7 +602,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$7</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -637,9 +637,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$5:$Q$5</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$5:$Q$5</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -691,7 +691,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$7:$Q$7</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$7:$Q$7</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="15"/>
@@ -752,7 +752,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$8</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -787,9 +787,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$5:$Q$5</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$5:$Q$5</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -841,7 +841,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$8:$Q$8</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$8:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="15"/>
@@ -896,7 +896,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$9</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -931,9 +931,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$5:$Q$5</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$5:$Q$5</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -985,7 +985,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$9:$Q$9</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$9:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1046,7 +1046,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$10</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1081,9 +1081,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$5:$Q$5</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$5:$Q$5</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -1135,7 +1135,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$10:$Q$10</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$10:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1178,7 +1178,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$11</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1213,9 +1213,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$5:$Q$5</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$5:$Q$5</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -1267,7 +1267,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$11:$Q$11</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$11:$Q$11</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1346,7 +1346,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1377,7 +1377,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1669464176"/>
@@ -1435,7 +1435,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1669594240"/>
@@ -1474,7 +1474,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1504,7 +1504,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1518,7 +1518,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1552,7 +1552,7 @@
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Valores do Etanol em Santa Rita do Sapucaí-MG entre 06/01/2020 e 06/03/2020</a:t>
+              <a:t>Preços do Etanol em Santa Rita do Sapucaí-MG entre 06/01/2020 e 06/03/2020</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" sz="1400" b="1" i="0">
               <a:solidFill>
@@ -1585,7 +1585,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1600,7 +1600,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$15</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1635,9 +1635,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$14:$O$14</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$14:$O$14</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -1683,7 +1683,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$15:$O$15</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$15:$O$15</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1738,7 +1738,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$16</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1773,9 +1773,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$14:$O$14</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$14:$O$14</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -1821,7 +1821,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$16:$O$16</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$16:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1876,7 +1876,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$17</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1911,9 +1911,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$14:$O$14</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$14:$O$14</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -1959,7 +1959,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$17:$O$17</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$17:$O$17</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2008,7 +2008,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$18</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2043,9 +2043,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$14:$O$14</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$14:$O$14</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -2091,7 +2091,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$18:$O$18</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$18:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2146,7 +2146,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$19</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2181,9 +2181,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$14:$O$14</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$14:$O$14</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -2229,7 +2229,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$19:$O$19</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$19:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2269,7 +2269,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pesquisa #01 - Valores'!$B$20</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2304,9 +2304,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$14:$O$14</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$14:$O$14</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43836</c:v>
@@ -2352,7 +2352,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pesquisa #01 - Valores'!$C$20:$O$20</c:f>
+              <c:f>'Pesquisa #01 - Preços'!$C$20:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>_-"R$"\ * #,##0.000_-;\-"R$"\ * #,##0.000_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2425,7 +2425,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2456,7 +2456,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1667319408"/>
@@ -2514,7 +2514,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1848667776"/>
@@ -2553,7 +2553,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2590,7 +2590,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3778,7 +3778,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4076,79 +4076,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F419A0E-6C88-4CD1-BCBF-61ABD01E164E}">
   <dimension ref="B2:Q46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:O20"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BO27" sqref="BO27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
-    <col min="3" max="17" width="15.7109375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.7109375" style="1"/>
+    <col min="1" max="1" width="2.6640625" style="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
+    <col min="3" max="17" width="15.6640625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="2.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-    </row>
-    <row r="3" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+    </row>
+    <row r="3" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-    </row>
-    <row r="4" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+    </row>
+    <row r="4" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-    </row>
-    <row r="5" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+    </row>
+    <row r="5" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>43896</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>4.859</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>5.0789999999999997</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>4.9489999999999998</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>5.0490000000000004</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>5.1989999999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
@@ -4471,25 +4471,25 @@
         <v>5.0590000000000002</v>
       </c>
     </row>
-    <row r="13" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+    </row>
+    <row r="14" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>43896</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>3.399</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>3.669</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>3.3889999999999998</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>3.5990000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>7</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>3.669</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
@@ -4773,163 +4773,163 @@
         <v>3.6589999999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
-    <row r="25" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
     </row>
-    <row r="26" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
     </row>
-    <row r="27" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
     </row>
-    <row r="28" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
     </row>
-    <row r="29" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
     </row>
-    <row r="30" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
     </row>
-    <row r="31" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
     </row>
-    <row r="32" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
     </row>
-    <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
     </row>
-    <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
     </row>
-    <row r="36" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
     </row>
-    <row r="37" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
     </row>
-    <row r="38" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
     </row>
-    <row r="39" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
       <c r="F39"/>
     </row>
-    <row r="40" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
     </row>
-    <row r="41" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
     </row>
-    <row r="42" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
       <c r="F42"/>
     </row>
-    <row r="43" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
       <c r="F43"/>
     </row>
-    <row r="44" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
       <c r="F44"/>
     </row>
-    <row r="45" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
       <c r="F45"/>
     </row>
-    <row r="46" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
@@ -4955,28 +4955,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBC412C-5268-4CB4-8635-53272D0623C4}">
   <dimension ref="B1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="50" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="10"/>
-    <col min="2" max="2" width="60.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="2.7109375" style="10"/>
+    <col min="1" max="1" width="2.6640625" style="10"/>
+    <col min="2" max="2" width="60.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="2.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+    <row r="1" spans="2:4" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
@@ -4987,8 +4987,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="10">
@@ -4998,456 +4998,456 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="10">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C6" s="10">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="10">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="11" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B10" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+    <row r="12" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="10">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+    <row r="14" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B14" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B17" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+    <row r="21" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B21" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+    <row r="22" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C22" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
+    <row r="23" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C23" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
+    <row r="24" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B24" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
+    <row r="25" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B25" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+    <row r="26" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+    <row r="27" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
+    <row r="28" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+    <row r="29" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
+    <row r="30" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="13" t="s">
+    <row r="31" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
+    <row r="32" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
+    <row r="33" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B33" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
+    <row r="34" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C34" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
+    <row r="35" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B35" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C35" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
+    <row r="36" spans="2:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C36" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B37" s="13" t="s">
+    <row r="37" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B37" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C37" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
+    <row r="38" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B38" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C38" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="13" t="s">
+    <row r="39" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B40" s="13" t="s">
+    <row r="40" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B41" s="13" t="s">
+    <row r="41" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="13" t="s">
+    <row r="42" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B42" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C42" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="13" t="s">
+    <row r="43" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B43" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C43" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="13" t="s">
+    <row r="44" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B44" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C44" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="13" t="s">
+    <row r="45" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B45" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C45" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="13" t="s">
+    <row r="46" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B46" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="13" t="s">
+    <row r="47" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B47" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C47" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="13" t="s">
+    <row r="48" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B48" s="11" t="s">
         <v>55</v>
       </c>
       <c r="C48" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="13" t="s">
+    <row r="49" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B49" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C49" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
+    <row r="50" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B50" s="11" t="s">
         <v>57</v>
       </c>
       <c r="C50" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" s="13" t="s">
+    <row r="51" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B51" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="13" t="s">
+    <row r="52" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B52" s="11" t="s">
         <v>61</v>
       </c>
       <c r="C52" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="13" t="s">
+    <row r="53" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B53" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C53" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
+    <row r="54" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B54" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C54" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="13" t="s">
+    <row r="55" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B55" s="11" t="s">
         <v>65</v>
       </c>
       <c r="C55" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="13" t="s">
+    <row r="56" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B56" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C56" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="13" t="s">
+    <row r="57" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B57" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C57" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="13" t="s">
+    <row r="58" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B58" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C58" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="13" t="s">
+    <row r="59" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B59" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C59" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B60" s="13" t="s">
+    <row r="60" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B60" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C60" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B61" s="13" t="s">
+    <row r="61" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B61" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C61" s="10">

</xml_diff>